<commit_message>
chore: fixed all known bugs
</commit_message>
<xml_diff>
--- a/saveTest.xlsx
+++ b/saveTest.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,26 +434,24 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>Grade</t>
         </is>
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Aarush</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>370</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>370</t>
+          <t>C1</t>
         </is>
       </c>
     </row>

</xml_diff>